<commit_message>
Signed-off-by: Manish Kumar <manish.kumar@softwareag.com>
</commit_message>
<xml_diff>
--- a/Asset.xlsx
+++ b/Asset.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\GitHubBack\PersonalDoc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAKUM\OneDrive - Software AG\Documents\Personal\PersGit\PersonalDo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DA934F-21D1-459E-8330-5394CBE9B910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20407634-255F-4F58-AFFD-1B0B656455D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B98719BE-EB54-4B9E-A858-358F680DEAF1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B98719BE-EB54-4B9E-A858-358F680DEAF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Holiday-21" sheetId="2" r:id="rId2"/>
-    <sheet name="Stock" sheetId="11" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
-    <sheet name="HPE-Dividend" sheetId="9" r:id="rId5"/>
-    <sheet name="ICICII" sheetId="4" r:id="rId6"/>
-    <sheet name="Sheet5" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet6" sheetId="8" r:id="rId8"/>
-    <sheet name="JNV" sheetId="10" r:id="rId9"/>
+    <sheet name="Budget" sheetId="13" r:id="rId2"/>
+    <sheet name="Interst-earn" sheetId="14" r:id="rId3"/>
+    <sheet name="Stock" sheetId="11" r:id="rId4"/>
+    <sheet name="RetirementPlan" sheetId="12" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
+    <sheet name="HPE-Dividend" sheetId="9" r:id="rId7"/>
+    <sheet name="ICICII" sheetId="4" r:id="rId8"/>
+    <sheet name="Sheet5" sheetId="7" r:id="rId9"/>
+    <sheet name="Sheet6" sheetId="8" r:id="rId10"/>
+    <sheet name="JNV" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="172">
   <si>
     <t>Gratuity</t>
   </si>
@@ -68,42 +70,6 @@
   </si>
   <si>
     <t>Liab</t>
-  </si>
-  <si>
-    <t>New Year’s Day</t>
-  </si>
-  <si>
-    <t>Public</t>
-  </si>
-  <si>
-    <t>Pongal /Makara Sankranti</t>
-  </si>
-  <si>
-    <t>Republic Day</t>
-  </si>
-  <si>
-    <t>Good Friday</t>
-  </si>
-  <si>
-    <t>Ugadi/Gudi Padwa</t>
-  </si>
-  <si>
-    <t>Id-ul-Fitr/Ramzan</t>
-  </si>
-  <si>
-    <t>Ganesh Chaturthi</t>
-  </si>
-  <si>
-    <t>Vijaya Dashami</t>
-  </si>
-  <si>
-    <t>Kannada Rajyotsava</t>
-  </si>
-  <si>
-    <t>Diwali</t>
-  </si>
-  <si>
-    <t>Guru Nanak Jayanti</t>
   </si>
   <si>
     <t>ULIP</t>
@@ -328,12 +294,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>yes Bank</t>
-  </si>
-  <si>
-    <t>Yes bank</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -356,13 +316,259 @@
   </si>
   <si>
     <t>Dividend share</t>
+  </si>
+  <si>
+    <t>2021-Dec</t>
+  </si>
+  <si>
+    <t>2022-Apr</t>
+  </si>
+  <si>
+    <t>2022-Dec</t>
+  </si>
+  <si>
+    <t>2023-Dec</t>
+  </si>
+  <si>
+    <t>2024-Dec</t>
+  </si>
+  <si>
+    <t>2 L</t>
+  </si>
+  <si>
+    <t>7 L</t>
+  </si>
+  <si>
+    <t>15 L</t>
+  </si>
+  <si>
+    <t>27 L</t>
+  </si>
+  <si>
+    <t>40L</t>
+  </si>
+  <si>
+    <t>3.5 L</t>
+  </si>
+  <si>
+    <t>4 L</t>
+  </si>
+  <si>
+    <t>Leaves</t>
+  </si>
+  <si>
+    <t>1L</t>
+  </si>
+  <si>
+    <t>1.5 L</t>
+  </si>
+  <si>
+    <t>2L</t>
+  </si>
+  <si>
+    <t>28L</t>
+  </si>
+  <si>
+    <t>29L + 2L (interest)</t>
+  </si>
+  <si>
+    <t>33 L</t>
+  </si>
+  <si>
+    <t>Liability</t>
+  </si>
+  <si>
+    <t>43 L</t>
+  </si>
+  <si>
+    <t>42 L</t>
+  </si>
+  <si>
+    <t>12 L (-ve)</t>
+  </si>
+  <si>
+    <t>ESPP</t>
+  </si>
+  <si>
+    <t>VPF</t>
+  </si>
+  <si>
+    <t>IMC</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>HL_1</t>
+  </si>
+  <si>
+    <t>HL_2</t>
+  </si>
+  <si>
+    <t>PL_1</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>Elect</t>
+  </si>
+  <si>
+    <t>Mob/Inter</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>Maid</t>
+  </si>
+  <si>
+    <t>Grocerry</t>
+  </si>
+  <si>
+    <t>Rest-Food</t>
+  </si>
+  <si>
+    <t>Commute</t>
+  </si>
+  <si>
+    <t>Invest_EMI</t>
+  </si>
+  <si>
+    <t>Loan</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Necessary</t>
+  </si>
+  <si>
+    <t>Earn</t>
+  </si>
+  <si>
+    <t>Man</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Invest</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Other-Earn</t>
+  </si>
+  <si>
+    <t>Gratuity(one-time)</t>
+  </si>
+  <si>
+    <t>HP-Sahare/Yr</t>
+  </si>
+  <si>
+    <t>Bonus/Yr</t>
+  </si>
+  <si>
+    <t>Interest/Quarter</t>
+  </si>
+  <si>
+    <t>Other-Expeses</t>
+  </si>
+  <si>
+    <t>School/Yr</t>
+  </si>
+  <si>
+    <t>LTA</t>
+  </si>
+  <si>
+    <t>One Year Projection</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>NftyBees</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Saving + share</t>
+  </si>
+  <si>
+    <t>FD</t>
+  </si>
+  <si>
+    <t>Surce</t>
+  </si>
+  <si>
+    <t>Fre</t>
+  </si>
+  <si>
+    <t>Amnt</t>
+  </si>
+  <si>
+    <t>Quarterly</t>
+  </si>
+  <si>
+    <t>Saving-M</t>
+  </si>
+  <si>
+    <t>Quaterly</t>
+  </si>
+  <si>
+    <t>Saving-A</t>
+  </si>
+  <si>
+    <t>EPF-A</t>
+  </si>
+  <si>
+    <t>EPF-M</t>
+  </si>
+  <si>
+    <t>Dividend-A</t>
+  </si>
+  <si>
+    <t>Shares/Quart</t>
+  </si>
+  <si>
+    <t>39 L</t>
+  </si>
+  <si>
+    <t>37 L</t>
+  </si>
+  <si>
+    <t>35L</t>
+  </si>
+  <si>
+    <t>14 L</t>
+  </si>
+  <si>
+    <t>5.5 L</t>
+  </si>
+  <si>
+    <t>45L</t>
+  </si>
+  <si>
+    <t>6.5L</t>
+  </si>
+  <si>
+    <t>58L</t>
+  </si>
+  <si>
+    <t>36 L</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,21 +576,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF494F69"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,14 +590,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -412,140 +599,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFDDDDDD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFD5D5D5"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFD5D5D5"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFDDDDDD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFD5D5D5"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFDDDDDD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFD5D5D5"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFD5D5D5"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFDDDDDD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFD5D5D5"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFDDDDDD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFD5D5D5"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFDDDDDD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFD5D5D5"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFD5D5D5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFD5D5D5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFD5D5D5"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFD5D5D5"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -554,6 +614,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,15 +931,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313F222D-A2F0-44C2-99C6-BFCFB386F73F}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -886,14 +949,17 @@
       <c r="E1">
         <v>2021</v>
       </c>
-      <c r="H1">
+      <c r="G1" s="8">
+        <v>44896</v>
+      </c>
+      <c r="K1">
         <v>2025</v>
       </c>
-      <c r="K1">
+      <c r="N1">
         <v>2030</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -909,20 +975,26 @@
       <c r="F2">
         <v>3.5</v>
       </c>
+      <c r="G2">
+        <v>12</v>
+      </c>
       <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="K2">
         <v>13</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <v>7</v>
       </c>
-      <c r="K2">
+      <c r="N2">
         <v>25</v>
       </c>
-      <c r="L2">
+      <c r="O2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -938,20 +1010,26 @@
       <c r="F3">
         <v>27</v>
       </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
       <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="K3">
         <v>35</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>50</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>70</v>
       </c>
-      <c r="L3">
+      <c r="O3">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -967,20 +1045,26 @@
       <c r="F4">
         <v>1</v>
       </c>
+      <c r="G4">
+        <v>5.5</v>
+      </c>
       <c r="H4">
+        <v>1.5</v>
+      </c>
+      <c r="K4">
         <v>10</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>8</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>20</v>
       </c>
-      <c r="L4">
+      <c r="O4">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -996,20 +1080,26 @@
       <c r="F5" s="1">
         <v>2</v>
       </c>
+      <c r="G5" s="1">
+        <v>20</v>
+      </c>
       <c r="H5" s="1">
+        <v>10</v>
+      </c>
+      <c r="K5" s="1">
         <v>50</v>
       </c>
-      <c r="I5" s="1">
+      <c r="L5" s="1">
         <v>25</v>
       </c>
-      <c r="K5" s="1">
+      <c r="N5" s="1">
         <v>110</v>
       </c>
-      <c r="L5" s="1">
+      <c r="O5" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1022,17 +1112,20 @@
       <c r="E6">
         <v>3.5</v>
       </c>
-      <c r="H6">
+      <c r="G6">
+        <v>3.5</v>
+      </c>
+      <c r="K6">
         <v>15</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <v>0</v>
       </c>
-      <c r="K6">
+      <c r="N6">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1048,20 +1141,26 @@
       <c r="F7">
         <v>11</v>
       </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
       <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
+        <v>20</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8">
         <f>SUM(B2:B7)</f>
         <v>33.5</v>
@@ -1078,24 +1177,32 @@
         <f>SUM(F2:F7)</f>
         <v>44.5</v>
       </c>
+      <c r="G8">
+        <f>SUM(G2:G7)</f>
+        <v>66</v>
+      </c>
       <c r="H8">
         <f>SUM(H2:H7)</f>
-        <v>123</v>
-      </c>
-      <c r="I8">
-        <f>SUM(I2:I7)</f>
-        <v>110</v>
+        <v>57.5</v>
       </c>
       <c r="K8">
         <f>SUM(K2:K7)</f>
-        <v>258</v>
+        <v>123</v>
       </c>
       <c r="L8">
         <f>SUM(L2:L7)</f>
+        <v>110</v>
+      </c>
+      <c r="N8">
+        <f>SUM(N2:N7)</f>
+        <v>258</v>
+      </c>
+      <c r="O8">
+        <f>SUM(O2:O7)</f>
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1110,6 +1217,352 @@
       </c>
       <c r="F11">
         <v>42</v>
+      </c>
+      <c r="G11">
+        <v>20</v>
+      </c>
+      <c r="H11">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D84A49-9C36-4472-90D9-A62418DCC544}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2">
+        <v>6.75</v>
+      </c>
+      <c r="C2">
+        <v>249.97</v>
+      </c>
+      <c r="D2">
+        <v>1.04</v>
+      </c>
+      <c r="E2">
+        <v>2.56</v>
+      </c>
+      <c r="H2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3">
+        <v>19.47</v>
+      </c>
+      <c r="C3">
+        <v>696.64</v>
+      </c>
+      <c r="D3">
+        <v>2.82</v>
+      </c>
+      <c r="E3">
+        <v>7.06</v>
+      </c>
+      <c r="H3">
+        <v>725.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4">
+        <v>18.09</v>
+      </c>
+      <c r="C4">
+        <v>692.02</v>
+      </c>
+      <c r="D4">
+        <v>2.82</v>
+      </c>
+      <c r="E4">
+        <v>7.06</v>
+      </c>
+      <c r="H4">
+        <v>720</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD66717-E9D5-4A5C-8E0C-BE94D20A6D16}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>2013</v>
+      </c>
+      <c r="B1">
+        <v>2014</v>
+      </c>
+      <c r="C1">
+        <v>2015</v>
+      </c>
+      <c r="D1">
+        <v>2016</v>
+      </c>
+      <c r="E1">
+        <v>2017</v>
+      </c>
+      <c r="F1">
+        <v>2003</v>
+      </c>
+      <c r="G1">
+        <v>2004</v>
+      </c>
+      <c r="H1">
+        <v>2005</v>
+      </c>
+      <c r="I1">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>80</v>
+      </c>
+      <c r="G2">
+        <v>30</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>39</v>
+      </c>
+      <c r="C3">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>81</v>
+      </c>
+      <c r="G3">
+        <v>45</v>
+      </c>
+      <c r="H3">
+        <v>14</v>
+      </c>
+      <c r="I3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>55</v>
+      </c>
+      <c r="C4">
+        <v>39</v>
+      </c>
+      <c r="D4">
+        <v>37</v>
+      </c>
+      <c r="H4">
+        <v>27</v>
+      </c>
+      <c r="I4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>56</v>
+      </c>
+      <c r="C5">
+        <v>45</v>
+      </c>
+      <c r="D5">
+        <v>54</v>
+      </c>
+      <c r="H5">
+        <v>49</v>
+      </c>
+      <c r="I5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>58</v>
+      </c>
+      <c r="C6">
+        <v>54</v>
+      </c>
+      <c r="D6">
+        <v>59</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>64</v>
+      </c>
+      <c r="B7">
+        <v>63</v>
+      </c>
+      <c r="C7">
+        <v>82</v>
+      </c>
+      <c r="D7">
+        <v>63</v>
+      </c>
+      <c r="H7">
+        <v>52</v>
+      </c>
+      <c r="I7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>68</v>
+      </c>
+      <c r="B8">
+        <v>74</v>
+      </c>
+      <c r="C8">
+        <v>96</v>
+      </c>
+      <c r="D8">
+        <v>72</v>
+      </c>
+      <c r="H8">
+        <v>54</v>
+      </c>
+      <c r="I8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <v>81</v>
+      </c>
+      <c r="C9">
+        <v>97</v>
+      </c>
+      <c r="D9">
+        <v>80</v>
+      </c>
+      <c r="H9">
+        <v>55</v>
+      </c>
+      <c r="I9">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>82</v>
+      </c>
+      <c r="I10">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>88</v>
+      </c>
+      <c r="I11">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1118,295 +1571,519 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60A2472-D9A4-4F2B-9C8D-446796283D73}">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA5D527-E862-4DF0-8806-FB0779C86A6C}">
+  <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2">
-        <v>44197</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" ht="75.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
-        <v>44210</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
-        <v>44222</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
-        <v>44288</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
-        <v>44299</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
-        <v>44330</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" ht="45.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
-        <v>44449</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
-        <v>44484</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
-        <v>44501</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
-        <v>44504</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9">
-        <v>44519</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B1" s="10">
+        <v>44764</v>
+      </c>
+      <c r="E1" s="10">
+        <v>44917</v>
+      </c>
+      <c r="L1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S1" t="s">
+        <v>74</v>
+      </c>
+      <c r="T1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>27294</v>
+      </c>
+      <c r="C2">
+        <v>27100</v>
+      </c>
+      <c r="E2">
+        <v>30000</v>
+      </c>
+      <c r="J2" t="s">
+        <v>118</v>
+      </c>
+      <c r="K2">
+        <v>45000</v>
+      </c>
+      <c r="M2" t="s">
+        <v>121</v>
+      </c>
+      <c r="N2">
+        <v>8000</v>
+      </c>
+      <c r="P2" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q2">
+        <v>10000</v>
+      </c>
+      <c r="S2" t="s">
+        <v>130</v>
+      </c>
+      <c r="T2">
+        <v>104000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="9">
+        <v>29734</v>
+      </c>
+      <c r="E3">
+        <v>33000</v>
+      </c>
+      <c r="J3" t="s">
+        <v>119</v>
+      </c>
+      <c r="K3">
+        <v>37000</v>
+      </c>
+      <c r="M3" t="s">
+        <v>122</v>
+      </c>
+      <c r="N3">
+        <v>3000</v>
+      </c>
+      <c r="P3" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q3">
+        <v>5000</v>
+      </c>
+      <c r="S3" t="s">
+        <v>131</v>
+      </c>
+      <c r="T3">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>11893</v>
+      </c>
+      <c r="C4">
+        <v>12000</v>
+      </c>
+      <c r="E4">
+        <v>13000</v>
+      </c>
+      <c r="J4" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4">
+        <v>22000</v>
+      </c>
+      <c r="M4" t="s">
+        <v>123</v>
+      </c>
+      <c r="N4">
+        <v>3000</v>
+      </c>
+      <c r="P4" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q4">
+        <v>2000</v>
+      </c>
+      <c r="S4" t="s">
+        <v>132</v>
+      </c>
+      <c r="T4">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5">
+        <v>7136</v>
+      </c>
+      <c r="E5">
+        <v>6000</v>
+      </c>
+      <c r="K5">
+        <f>SUM(K2:K4)</f>
+        <v>104000</v>
+      </c>
+      <c r="M5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N5">
+        <v>2000</v>
+      </c>
+      <c r="T5">
+        <f>SUM(T2:T4)</f>
+        <v>151000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6">
+        <v>15534</v>
+      </c>
+      <c r="C6">
+        <v>16000</v>
+      </c>
+      <c r="E6">
+        <v>16000</v>
+      </c>
+      <c r="M6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N6">
+        <v>2000</v>
+      </c>
+      <c r="Q6">
+        <f>SUM(Q2:Q5)</f>
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7">
+        <v>6000</v>
+      </c>
+      <c r="C7">
+        <v>3000</v>
+      </c>
+      <c r="E7">
+        <v>6000</v>
+      </c>
+      <c r="M7" t="s">
+        <v>129</v>
+      </c>
+      <c r="N7">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N8">
+        <f>SUM(N2:N7)</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9">
+        <f>SUM(B2:B8)</f>
+        <v>97591</v>
+      </c>
+      <c r="C9">
+        <f>SUM(C2:C8)</f>
+        <v>58100</v>
+      </c>
+      <c r="E9">
+        <f>SUM(E2:E8)</f>
+        <v>104000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15">
+        <v>190000</v>
+      </c>
+      <c r="C15">
+        <v>100000</v>
+      </c>
+      <c r="D15">
+        <v>45000</v>
+      </c>
+      <c r="E15">
+        <v>40000</v>
+      </c>
+      <c r="F15">
+        <v>50000</v>
+      </c>
+      <c r="I15" t="s">
+        <v>136</v>
+      </c>
+      <c r="J15">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16">
+        <v>155000</v>
+      </c>
+      <c r="C16">
+        <v>50000</v>
+      </c>
+      <c r="D16">
+        <v>75000</v>
+      </c>
+      <c r="E16">
+        <v>50000</v>
+      </c>
+      <c r="F16">
+        <v>50000</v>
+      </c>
+      <c r="I16" t="s">
+        <v>137</v>
+      </c>
+      <c r="J16">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <f>SUM(B15:B16)</f>
+        <v>345000</v>
+      </c>
+      <c r="C17">
+        <f>SUM(C15:C16)</f>
+        <v>150000</v>
+      </c>
+      <c r="D17">
+        <f>SUM(D15:D16)</f>
+        <v>120000</v>
+      </c>
+      <c r="E17">
+        <f>SUM(E15:E16)</f>
+        <v>90000</v>
+      </c>
+      <c r="F17">
+        <f>SUM(F15:F16)</f>
+        <v>100000</v>
+      </c>
+      <c r="I17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J18">
+        <v>700000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>10000</v>
+      </c>
+      <c r="C20">
+        <v>400000</v>
+      </c>
+      <c r="D20">
+        <v>700000</v>
+      </c>
+      <c r="E20">
+        <v>1400000</v>
+      </c>
+      <c r="I20" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20">
+        <f>SUM(J15:J19)</f>
+        <v>4600000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>143</v>
+      </c>
+      <c r="B22" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>400000</v>
+      </c>
+      <c r="C23">
+        <v>100000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C0DB57-45C7-4504-A33B-E6498916F6CF}">
-  <dimension ref="A1:D20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCABD12-3059-44FD-B3B8-E009C35DB12C}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>153</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6">
-        <v>975</v>
+        <v>160</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
       </c>
       <c r="C6">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7">
-        <v>800</v>
+        <v>161</v>
+      </c>
+      <c r="B7" t="s">
+        <v>155</v>
       </c>
       <c r="C7">
-        <v>15.85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8">
-        <v>1300</v>
+        <v>161</v>
+      </c>
+      <c r="B8" t="s">
+        <v>162</v>
       </c>
       <c r="C8">
-        <v>15.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9">
-        <v>1500</v>
-      </c>
-      <c r="C9">
-        <v>15.55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10">
-        <v>900</v>
-      </c>
-      <c r="C10">
-        <v>14.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B11">
-        <v>1500</v>
-      </c>
-      <c r="C11">
-        <v>13.85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12">
-        <v>1000</v>
-      </c>
-      <c r="C12">
-        <v>13.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20">
-        <f>SUM(B6:B19)</f>
-        <v>7975</v>
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -1415,6 +2092,266 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C0DB57-45C7-4504-A33B-E6498916F6CF}">
+  <dimension ref="A1:N20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3">
+        <v>300</v>
+      </c>
+      <c r="H3">
+        <v>186.36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>375</v>
+      </c>
+      <c r="H4">
+        <v>185.24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>500</v>
+      </c>
+      <c r="H5">
+        <v>183.66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>350</v>
+      </c>
+      <c r="H6">
+        <v>182.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>400</v>
+      </c>
+      <c r="H7">
+        <v>178.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>400</v>
+      </c>
+      <c r="H8">
+        <v>171.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <v>170.15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <f>SUM(G3:G13)</f>
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <f>SUM(B6:B19)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50D8B70-34DA-479D-99A1-745595DA7655}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" t="s">
+        <v>164</v>
+      </c>
+      <c r="F6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD21665A-23F8-44A6-BBBB-89F49F8AA360}">
   <dimension ref="A1:N7"/>
   <sheetViews>
@@ -1425,61 +2362,61 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="3" customWidth="1"/>
     <col min="14" max="14" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="N1" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>29</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C2">
         <v>20000</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="2">
         <v>39120</v>
       </c>
       <c r="E2">
@@ -1491,7 +2428,7 @@
       <c r="G2">
         <v>800</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="4">
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="K2">
@@ -1503,15 +2440,15 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>34</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="C3">
         <v>20000</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="2">
         <v>39407</v>
       </c>
       <c r="E3">
@@ -1523,11 +2460,11 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="4">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J3" s="13" t="s">
-        <v>36</v>
+      <c r="J3" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="K3">
         <v>4</v>
@@ -1535,15 +2472,15 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>38</v>
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C4">
         <v>25000</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="2">
         <v>39829</v>
       </c>
       <c r="E4">
@@ -1555,11 +2492,11 @@
       <c r="H4">
         <v>760</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="4">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J4" s="13" t="s">
-        <v>39</v>
+      <c r="J4" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="K4">
         <v>100</v>
@@ -1567,36 +2504,36 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="4">
         <v>1.35E-2</v>
       </c>
-      <c r="J6" s="13" t="s">
-        <v>45</v>
+      <c r="J6" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="15">
+        <v>34</v>
+      </c>
+      <c r="G7" s="5">
         <v>0.05</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="4">
         <v>1.35E-2</v>
       </c>
-      <c r="J7" s="13" t="s">
-        <v>36</v>
+      <c r="J7" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1605,45 +2542,46 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBFE8F9A-D870-4289-9775-9C157F06B43E}">
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="E1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="H1" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="I1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1913,7 +2851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D360A2-36FA-41FE-B861-16B8902DB39F}">
   <dimension ref="A1:L16"/>
   <sheetViews>
@@ -1928,28 +2866,28 @@
         <v>6736</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="H1">
         <v>4441535</v>
       </c>
       <c r="I1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="K1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="L1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -2180,7 +3118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7004B924-DDAE-4B12-A905-ADFA4DBF16C6}">
   <dimension ref="A1:G17"/>
   <sheetViews>
@@ -2200,13 +3138,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="F1">
         <v>44</v>
@@ -2217,12 +3155,12 @@
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="14">
+        <v>37</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="4">
         <v>3.2500000000000001E-2</v>
       </c>
       <c r="D2">
@@ -2232,20 +3170,20 @@
         <v>1.5</v>
       </c>
       <c r="G2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>30000</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="6">
         <v>200000</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="6">
         <v>200000</v>
       </c>
       <c r="F3">
@@ -2257,21 +3195,21 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <v>300000</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="6">
         <v>2000000</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="6">
         <v>2000000</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>37500</v>
@@ -2279,69 +3217,69 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
         <v>56</v>
       </c>
-      <c r="B9" t="s">
-        <v>68</v>
-      </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F10">
         <v>4</v>
@@ -2352,7 +3290,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C11">
         <v>2000</v>
@@ -2366,53 +3304,53 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="15">
+        <v>49</v>
+      </c>
+      <c r="D12" s="5">
         <v>0.05</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="5">
         <v>0.03</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="5">
         <v>0.04</v>
       </c>
       <c r="G12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="14">
+        <v>60</v>
+      </c>
+      <c r="C13" s="4">
         <v>1.35E-2</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="4">
         <v>1.35E-2</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="4">
         <v>1.35E-2</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="4">
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="G13" s="14" t="s">
-        <v>77</v>
+      <c r="G13" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C14">
         <v>1200</v>
@@ -2429,27 +3367,27 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D15">
         <v>2000</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="6">
         <v>2000</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>75</v>
+      <c r="F15" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>73</v>
+      <c r="A17" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="C17">
         <v>5500</v>
@@ -2457,8 +3395,8 @@
       <c r="D17">
         <v>6000</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>74</v>
+      <c r="E17" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="F17">
         <v>8750</v>
@@ -2472,342 +3410,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D84A49-9C36-4472-90D9-A62418DCC544}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2">
-        <v>6.75</v>
-      </c>
-      <c r="C2">
-        <v>249.97</v>
-      </c>
-      <c r="D2">
-        <v>1.04</v>
-      </c>
-      <c r="E2">
-        <v>2.56</v>
-      </c>
-      <c r="H2">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3">
-        <v>19.47</v>
-      </c>
-      <c r="C3">
-        <v>696.64</v>
-      </c>
-      <c r="D3">
-        <v>2.82</v>
-      </c>
-      <c r="E3">
-        <v>7.06</v>
-      </c>
-      <c r="H3">
-        <v>725.99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4">
-        <v>18.09</v>
-      </c>
-      <c r="C4">
-        <v>692.02</v>
-      </c>
-      <c r="D4">
-        <v>2.82</v>
-      </c>
-      <c r="E4">
-        <v>7.06</v>
-      </c>
-      <c r="H4">
-        <v>720</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD66717-E9D5-4A5C-8E0C-BE94D20A6D16}">
-  <dimension ref="A1:I13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>2013</v>
-      </c>
-      <c r="B1">
-        <v>2014</v>
-      </c>
-      <c r="C1">
-        <v>2015</v>
-      </c>
-      <c r="D1">
-        <v>2016</v>
-      </c>
-      <c r="E1">
-        <v>2017</v>
-      </c>
-      <c r="F1">
-        <v>2003</v>
-      </c>
-      <c r="G1">
-        <v>2004</v>
-      </c>
-      <c r="H1">
-        <v>2005</v>
-      </c>
-      <c r="I1">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>21</v>
-      </c>
-      <c r="C2">
-        <v>19</v>
-      </c>
-      <c r="D2">
-        <v>8</v>
-      </c>
-      <c r="F2">
-        <v>80</v>
-      </c>
-      <c r="G2">
-        <v>30</v>
-      </c>
-      <c r="H2">
-        <v>4</v>
-      </c>
-      <c r="I2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>39</v>
-      </c>
-      <c r="C3">
-        <v>36</v>
-      </c>
-      <c r="D3">
-        <v>25</v>
-      </c>
-      <c r="F3">
-        <v>81</v>
-      </c>
-      <c r="G3">
-        <v>45</v>
-      </c>
-      <c r="H3">
-        <v>14</v>
-      </c>
-      <c r="I3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>47</v>
-      </c>
-      <c r="B4">
-        <v>55</v>
-      </c>
-      <c r="C4">
-        <v>39</v>
-      </c>
-      <c r="D4">
-        <v>37</v>
-      </c>
-      <c r="H4">
-        <v>27</v>
-      </c>
-      <c r="I4">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>48</v>
-      </c>
-      <c r="B5">
-        <v>56</v>
-      </c>
-      <c r="C5">
-        <v>45</v>
-      </c>
-      <c r="D5">
-        <v>54</v>
-      </c>
-      <c r="H5">
-        <v>49</v>
-      </c>
-      <c r="I5">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>60</v>
-      </c>
-      <c r="B6">
-        <v>58</v>
-      </c>
-      <c r="C6">
-        <v>54</v>
-      </c>
-      <c r="D6">
-        <v>59</v>
-      </c>
-      <c r="H6">
-        <v>50</v>
-      </c>
-      <c r="I6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>64</v>
-      </c>
-      <c r="B7">
-        <v>63</v>
-      </c>
-      <c r="C7">
-        <v>82</v>
-      </c>
-      <c r="D7">
-        <v>63</v>
-      </c>
-      <c r="H7">
-        <v>52</v>
-      </c>
-      <c r="I7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>68</v>
-      </c>
-      <c r="B8">
-        <v>74</v>
-      </c>
-      <c r="C8">
-        <v>96</v>
-      </c>
-      <c r="D8">
-        <v>72</v>
-      </c>
-      <c r="H8">
-        <v>54</v>
-      </c>
-      <c r="I8">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>70</v>
-      </c>
-      <c r="B9">
-        <v>81</v>
-      </c>
-      <c r="C9">
-        <v>97</v>
-      </c>
-      <c r="D9">
-        <v>80</v>
-      </c>
-      <c r="H9">
-        <v>55</v>
-      </c>
-      <c r="I9">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D10">
-        <v>82</v>
-      </c>
-      <c r="I10">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D11">
-        <v>88</v>
-      </c>
-      <c r="I11">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I12">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I13">
-        <v>85</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{ee9ddd37-01c2-47a1-893c-5c0bdc1f6d39}" enabled="1" method="Privileged" siteId="{d9662eb9-ad98-4e74-a8a2-04ed5d544db6}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>